<commit_message>
Feat: Added animals in the menu screen
</commit_message>
<xml_diff>
--- a/Drone Control in VR - Testing data RV2324.xlsx
+++ b/Drone Control in VR - Testing data RV2324.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berna\Desktop\RVirtual2425\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA9CA182-505D-4D7B-B939-F8B8C7A95951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC293BA9-2426-49C5-92B1-0D34EDAB42FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5C40AECF-C350-4196-A695-ACF50D0E7074}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5C40AECF-C350-4196-A695-ACF50D0E7074}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -62,19 +62,19 @@
     <t>Hand</t>
   </si>
   <si>
-    <t>SheepWhite</t>
-  </si>
-  <si>
-    <t>CowBlW</t>
-  </si>
-  <si>
     <t>Pig</t>
   </si>
   <si>
-    <t>DuckWhite</t>
-  </si>
-  <si>
-    <t>ChickenBrown</t>
+    <t>Sheep</t>
+  </si>
+  <si>
+    <t>Chicken</t>
+  </si>
+  <si>
+    <t>Cow</t>
+  </si>
+  <si>
+    <t>Duck</t>
   </si>
 </sst>
 </file>
@@ -128,11 +128,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -144,14 +141,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -490,655 +481,653 @@
   <dimension ref="B2:J34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="G2" s="1" t="s">
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="G2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>1</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E4">
         <v>23.54035</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <v>2</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="I4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J4">
         <v>40.140729999999998</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E5">
         <v>35.38062</v>
       </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
       <c r="I5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="J5">
         <v>71.160070000000005</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E6">
         <v>47.900910000000003</v>
       </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
       <c r="I6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J6">
         <v>108.27379999999999</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E7">
         <v>58.541150000000002</v>
       </c>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
       <c r="I7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J7">
         <v>150.8954</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="3" t="s">
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="2">
+        <v>78.438850000000002</v>
+      </c>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" s="2">
+        <v>259.65589999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="3">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
         <v>11</v>
-      </c>
-      <c r="E8" s="3">
-        <v>78.438850000000002</v>
-      </c>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J8" s="3">
-        <v>259.65589999999997</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="4">
-        <v>1</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" t="s">
-        <v>9</v>
       </c>
       <c r="E9">
         <v>9.5600280000000009</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="3">
         <v>2</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="3" t="s">
         <v>7</v>
       </c>
       <c r="I9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J9">
         <v>5.5199949999999998</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
       <c r="D10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E10">
         <v>19.120249999999999</v>
       </c>
-      <c r="G10" s="5"/>
-      <c r="H10" s="7"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
       <c r="I10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J10">
         <v>14.940149999999999</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
       <c r="D11" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E11">
         <v>27.980450000000001</v>
       </c>
-      <c r="G11" s="5"/>
-      <c r="H11" s="7"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
       <c r="I11" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="J11">
         <v>31.900539999999999</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
       <c r="D12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E12">
         <v>40.080730000000003</v>
       </c>
-      <c r="G12" s="5"/>
-      <c r="H12" s="7"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
       <c r="I12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J12">
         <v>161.71770000000001</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="3" t="s">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="2">
+        <v>47.760899999999999</v>
+      </c>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="3">
-        <v>47.760899999999999</v>
-      </c>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J13" s="3">
+      <c r="J13" s="2">
         <v>300.01369999999997</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="8">
+      <c r="B14" s="3">
         <v>3</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E14">
         <v>20.640280000000001</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="3">
         <v>4</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="H14" s="3" t="s">
         <v>6</v>
       </c>
       <c r="I14" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="J14">
         <v>23.940359999999998</v>
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
       <c r="D15" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E15">
         <v>38.500689999999999</v>
       </c>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
       <c r="I15" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J15">
         <v>39.220709999999997</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
       <c r="D16" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E16">
         <v>48.84093</v>
       </c>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
       <c r="I16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J16">
         <v>53.02102</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
       <c r="D17" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E17">
         <v>90.336849999999998</v>
       </c>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
       <c r="I17" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J17">
         <v>91.456670000000003</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
       <c r="D18" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E18">
         <v>124.8111</v>
       </c>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J18" s="3">
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J18" s="2">
         <v>264.9529</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="4">
+      <c r="B19" s="3">
         <v>3</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" s="2">
+      <c r="D19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="1">
         <v>9.2800220000000007</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G19" s="3">
         <v>4</v>
       </c>
-      <c r="H19" s="4" t="s">
+      <c r="H19" s="3" t="s">
         <v>7</v>
       </c>
       <c r="I19" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J19">
         <v>17.220199999999998</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
       <c r="D20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E20">
         <v>33.30057</v>
       </c>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
       <c r="I20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J20">
         <v>23.760349999999999</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
       <c r="D21" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E21">
         <v>50.62097</v>
       </c>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
       <c r="I21" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J21">
         <v>31.160520000000002</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
       <c r="D22" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E22">
         <v>66.280889999999999</v>
       </c>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
       <c r="I22" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="J22">
         <v>62.14123</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" s="3">
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="2">
         <v>86.057569999999998</v>
       </c>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J23" s="3">
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J23" s="2">
         <v>107.194</v>
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24" s="8">
+      <c r="B24" s="3">
         <v>5</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D24" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E24">
         <v>15.580170000000001</v>
       </c>
-      <c r="G24" s="8">
+      <c r="G24" s="3">
         <v>6</v>
       </c>
-      <c r="H24" s="8" t="s">
+      <c r="H24" s="3" t="s">
         <v>6</v>
       </c>
       <c r="I24" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="J24">
         <v>30.860520000000001</v>
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
       <c r="D25" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E25">
         <v>23.360340000000001</v>
       </c>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
       <c r="I25" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J25">
         <v>52.301009999999998</v>
       </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
       <c r="D26" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E26">
         <v>42.060769999999998</v>
       </c>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
       <c r="I26" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J26">
         <v>62.661239999999999</v>
       </c>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B27" s="9"/>
-      <c r="C27" s="9"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
       <c r="D27" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E27">
         <v>71.300049999999999</v>
       </c>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
       <c r="I27" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J27">
         <v>97.855590000000007</v>
       </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
       <c r="D28" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E28">
         <v>92.196539999999999</v>
       </c>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
       <c r="I28" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J28">
         <v>139.63300000000001</v>
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B29" s="4">
+      <c r="B29" s="3">
         <v>5</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E29" s="2">
+      <c r="D29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" s="1">
         <v>9.5986600000000006</v>
       </c>
-      <c r="G29" s="4">
+      <c r="G29" s="3">
         <v>6</v>
       </c>
-      <c r="H29" s="4" t="s">
+      <c r="H29" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I29" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J29" s="2">
+      <c r="I29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J29" s="1">
         <v>13.36012</v>
       </c>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
       <c r="D30" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E30">
         <v>40.613399999999999</v>
       </c>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
       <c r="I30" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J30">
         <v>29.30048</v>
       </c>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
       <c r="D31" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E31">
         <v>66.712400000000002</v>
       </c>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
       <c r="I31" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="J31">
         <v>50.200960000000002</v>
       </c>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
       <c r="D32" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E32">
         <v>86.476600000000005</v>
       </c>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
       <c r="I32" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J32">
         <v>62.741250000000001</v>
       </c>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E33" s="3">
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="2">
         <v>104.9606</v>
       </c>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
       <c r="I33" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J33">
         <v>72.499849999999995</v>
       </c>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B24:B28"/>
-    <mergeCell ref="C24:C28"/>
-    <mergeCell ref="B29:B33"/>
-    <mergeCell ref="C29:C33"/>
-    <mergeCell ref="G24:G28"/>
-    <mergeCell ref="H24:H28"/>
-    <mergeCell ref="G29:G33"/>
-    <mergeCell ref="H29:H33"/>
-    <mergeCell ref="B19:B23"/>
-    <mergeCell ref="C19:C23"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="B14:B18"/>
+    <mergeCell ref="C14:C18"/>
+    <mergeCell ref="C9:C13"/>
+    <mergeCell ref="B9:B13"/>
+    <mergeCell ref="B4:B8"/>
+    <mergeCell ref="C4:C8"/>
     <mergeCell ref="G9:G13"/>
     <mergeCell ref="H9:H13"/>
     <mergeCell ref="H4:H8"/>
@@ -1147,14 +1136,16 @@
     <mergeCell ref="H19:H23"/>
     <mergeCell ref="H14:H18"/>
     <mergeCell ref="G14:G18"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="B14:B18"/>
-    <mergeCell ref="C14:C18"/>
-    <mergeCell ref="C9:C13"/>
-    <mergeCell ref="B9:B13"/>
-    <mergeCell ref="B4:B8"/>
-    <mergeCell ref="C4:C8"/>
+    <mergeCell ref="H24:H28"/>
+    <mergeCell ref="G29:G33"/>
+    <mergeCell ref="H29:H33"/>
+    <mergeCell ref="B19:B23"/>
+    <mergeCell ref="C19:C23"/>
+    <mergeCell ref="B24:B28"/>
+    <mergeCell ref="C24:C28"/>
+    <mergeCell ref="B29:B33"/>
+    <mergeCell ref="C29:C33"/>
+    <mergeCell ref="G24:G28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>